<commit_message>
added odeint original tried to make iterative odeint work
</commit_message>
<xml_diff>
--- a/GroundDataExample4.xlsx
+++ b/GroundDataExample4.xlsx
@@ -383,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,7 +402,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>SIN(A2)</f>
+        <f>SIN(2*A2)</f>
         <v>0</v>
       </c>
     </row>
@@ -411,8 +411,8 @@
         <v>0.1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B66" si="0">SIN(A3)</f>
-        <v>9.9833416646828155E-2</v>
+        <f t="shared" ref="B3:B66" si="0">SIN(2*A3)</f>
+        <v>0.19866933079506122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -421,7 +421,7 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>0.19866933079506122</v>
+        <v>0.38941834230865052</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -430,7 +430,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0.29552020666133955</v>
+        <v>0.56464247339503537</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -439,7 +439,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>0.38941834230865052</v>
+        <v>0.71735609089952279</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -448,7 +448,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>0.47942553860420301</v>
+        <v>0.8414709848078965</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -457,7 +457,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0.56464247339503537</v>
+        <v>0.93203908596722629</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -466,7 +466,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>0.64421768723769102</v>
+        <v>0.98544972998846014</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -475,7 +475,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>0.71735609089952279</v>
+        <v>0.99957360304150511</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,7 +484,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>0.78332690962748341</v>
+        <v>0.97384763087819515</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -493,7 +493,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>0.8414709848078965</v>
+        <v>0.90929742682568171</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -502,7 +502,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>0.89120736006143542</v>
+        <v>0.80849640381959009</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -511,7 +511,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>0.93203908596722629</v>
+        <v>0.67546318055115095</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -520,7 +520,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>0.96355818541719296</v>
+        <v>0.51550137182146416</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>0.98544972998846014</v>
+        <v>0.33498815015590511</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>0.99749498660405445</v>
+        <v>0.14112000805986721</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -547,7 +547,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>0.99957360304150511</v>
+        <v>-5.8374143427580086E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>0.99166481045246857</v>
+        <v>-0.25554110202683122</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>0.97384763087819515</v>
+        <v>-0.44252044329485246</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>0.94630008768741447</v>
+        <v>-0.61185789094271892</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -583,7 +583,7 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>0.90929742682568171</v>
+        <v>-0.7568024953079282</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -592,7 +592,7 @@
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>0.86320936664887371</v>
+        <v>-0.87157577241358819</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>0.80849640381959009</v>
+        <v>-0.95160207388951601</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -610,7 +610,7 @@
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>0.74570521217672026</v>
+        <v>-0.99369100363346441</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -619,7 +619,7 @@
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>0.67546318055115095</v>
+        <v>-0.99616460883584068</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>0.59847214410395655</v>
+        <v>-0.95892427466313845</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>0.51550137182146416</v>
+        <v>-0.88345465572015314</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>0.42737988023382978</v>
+        <v>-0.77276448755598715</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -655,7 +655,7 @@
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>0.33498815015590511</v>
+        <v>-0.63126663787232162</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>0.23924932921398243</v>
+        <v>-0.46460217941375737</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>0.14112000805986721</v>
+        <v>-0.27941549819892586</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -682,7 +682,7 @@
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>4.1580662433290491E-2</v>
+        <v>-8.3089402817496397E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -691,7 +691,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>-5.8374143427580086E-2</v>
+        <v>0.11654920485049364</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>-0.15774569414324821</v>
+        <v>0.31154136351337786</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>-0.25554110202683122</v>
+        <v>0.49411335113860816</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>-0.35078322768961984</v>
+        <v>0.65698659871878906</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>-0.44252044329485246</v>
+        <v>0.79366786384915311</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -736,7 +736,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>-0.5298361409084934</v>
+        <v>0.89870809581162692</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>-0.61185789094271892</v>
+        <v>0.96791967203148632</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -754,7 +754,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>-0.68776615918397377</v>
+        <v>0.99854334537460498</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>-0.7568024953079282</v>
+        <v>0.98935824662338179</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>-0.81827711106441026</v>
+        <v>0.94073055667977312</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -781,7 +781,7 @@
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>-0.87157577241358819</v>
+        <v>0.85459890808828043</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>-0.9161659367494549</v>
+        <v>0.73439709787411334</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>-0.95160207388951601</v>
+        <v>0.58491719289176169</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>-0.97753011766509701</v>
+        <v>0.41211848524175659</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -817,7 +817,7 @@
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>-0.99369100363346441</v>
+        <v>0.22288991410024764</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -826,7 +826,7 @@
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>-0.99992325756410083</v>
+        <v>2.4775425453357765E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>-0.99616460883584068</v>
+        <v>-0.17432678122297965</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>-0.98245261262433248</v>
+        <v>-0.36647912925192838</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -853,7 +853,7 @@
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>-0.95892427466313845</v>
+        <v>-0.54402111088936977</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>-0.92581468232773245</v>
+        <v>-0.69987468759354232</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -871,7 +871,7 @@
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>-0.88345465572015314</v>
+        <v>-0.82782646908565372</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>-0.83226744222390125</v>
+        <v>-0.92277542161280657</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>-0.77276448755598715</v>
+        <v>-0.98093623006649155</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -898,7 +898,7 @@
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>-0.70554032557039192</v>
+        <v>-0.99999020655070348</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -907,7 +907,7 @@
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>-0.63126663787232162</v>
+        <v>-0.9791777291513174</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -916,7 +916,7 @@
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>-0.55068554259763758</v>
+        <v>-0.91932852566467571</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -925,7 +925,7 @@
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>-0.46460217941375737</v>
+        <v>-0.82282859496870886</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -934,7 +934,7 @@
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>-0.37387666483023602</v>
+        <v>-0.69352508477712238</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>-0.27941549819892586</v>
+        <v>-0.53657291800043494</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -952,7 +952,7 @@
       </c>
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>-0.18216250427209588</v>
+        <v>-0.35822928223682871</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>-8.3089402817496397E-2</v>
+        <v>-0.16560417544830941</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>1.6813900484349713E-2</v>
+        <v>3.3623047221136695E-2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
       </c>
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>0.11654920485049364</v>
+        <v>0.23150982510153895</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -987,8 +987,8 @@
         <v>6.5</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B102" si="1">SIN(A67)</f>
-        <v>0.21511998808781552</v>
+        <f t="shared" ref="B67:B102" si="1">SIN(2*A67)</f>
+        <v>0.42016703682664092</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -997,7 +997,7 @@
       </c>
       <c r="B68">
         <f t="shared" si="1"/>
-        <v>0.31154136351337786</v>
+        <v>0.59207351470722303</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="B69">
         <f t="shared" si="1"/>
-        <v>0.4048499206165983</v>
+        <v>0.74037588995244863</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="B70">
         <f t="shared" si="1"/>
-        <v>0.49411335113860816</v>
+        <v>0.85916181485649579</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="B71">
         <f t="shared" si="1"/>
-        <v>0.57843976438820011</v>
+        <v>0.94369566944410477</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="B72">
         <f t="shared" si="1"/>
-        <v>0.65698659871878906</v>
+        <v>0.99060735569487035</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="B73">
         <f t="shared" si="1"/>
-        <v>0.72896904012587593</v>
+        <v>0.99802665271636171</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="B74">
         <f t="shared" si="1"/>
-        <v>0.79366786384915311</v>
+        <v>0.96565777654927742</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="B75">
         <f t="shared" si="1"/>
-        <v>0.8504366206285644</v>
+        <v>0.89479117214050419</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B76">
         <f t="shared" si="1"/>
-        <v>0.89870809581162692</v>
+        <v>0.78825206737531628</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="B77">
         <f t="shared" si="1"/>
-        <v>0.9379999767747389</v>
+        <v>0.65028784015711683</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B78">
         <f t="shared" si="1"/>
-        <v>0.96791967203148632</v>
+        <v>0.48639868885379967</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="B79">
         <f t="shared" si="1"/>
-        <v>0.98816823387700037</v>
+        <v>0.30311835674570226</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="B80">
         <f t="shared" si="1"/>
-        <v>0.99854334537460498</v>
+        <v>0.10775365229944406</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B81">
         <f t="shared" si="1"/>
-        <v>0.99894134183977201</v>
+        <v>-9.1906850227681636E-2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B82">
         <f t="shared" si="1"/>
-        <v>0.98935824662338179</v>
+        <v>-0.2879033166650653</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="B83">
         <f t="shared" si="1"/>
-        <v>0.9698898108450863</v>
+        <v>-0.47242198639846616</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="B84">
         <f t="shared" si="1"/>
-        <v>0.94073055667977312</v>
+        <v>-0.63810668234794743</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="B85">
         <f t="shared" si="1"/>
-        <v>0.90217183375629328</v>
+        <v>-0.77835207853429844</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B86">
         <f t="shared" si="1"/>
-        <v>0.85459890808828043</v>
+        <v>-0.88756703358150457</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B87">
         <f t="shared" si="1"/>
-        <v>0.79848711262349026</v>
+        <v>-0.96139749187955681</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B88">
         <f t="shared" si="1"/>
-        <v>0.73439709787411334</v>
+        <v>-0.99690006604159609</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="B89">
         <f t="shared" si="1"/>
-        <v>0.66296923008218334</v>
+        <v>-0.99265938047063318</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="B90">
         <f t="shared" si="1"/>
-        <v>0.58491719289176169</v>
+        <v>-0.94884449791812397</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="B91">
         <f t="shared" si="1"/>
-        <v>0.50102085645788463</v>
+        <v>-0.86720217948558131</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B92">
         <f t="shared" si="1"/>
-        <v>0.41211848524175659</v>
+        <v>-0.75098724677167605</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="B93">
         <f t="shared" si="1"/>
-        <v>0.31909836234935213</v>
+        <v>-0.60483282240628411</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B94">
         <f t="shared" si="1"/>
-        <v>0.22288991410024764</v>
+        <v>-0.43456562207189675</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="B95">
         <f t="shared" si="1"/>
-        <v>0.12445442350706171</v>
+        <v>-0.24697366173662089</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="B96">
         <f t="shared" si="1"/>
-        <v>2.4775425453357765E-2</v>
+        <v>-4.9535640878367419E-2</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="B97">
         <f t="shared" si="1"/>
-        <v>-7.5151120461809301E-2</v>
+        <v>0.14987720966295234</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="B98">
         <f t="shared" si="1"/>
-        <v>-0.17432678122297965</v>
+        <v>0.34331492881989539</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="B99">
         <f t="shared" si="1"/>
-        <v>-0.27176062641094245</v>
+        <v>0.52306576515769643</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="B100">
         <f t="shared" si="1"/>
-        <v>-0.36647912925192838</v>
+        <v>0.6819636200681356</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="B101">
         <f t="shared" si="1"/>
-        <v>-0.45753589377532133</v>
+        <v>0.81367373750710537</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B102">
         <f t="shared" si="1"/>
-        <v>-0.54402111088936977</v>
+        <v>0.91294525072762767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>